<commit_message>
Added IBS Test Data and changed downsampling to 8kHz
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Mounted(abcd@10_SIDEStrong-Best)/Median_Pulse_Widths.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Mounted(abcd@10_SIDEStrong-Best)/Median_Pulse_Widths.xlsx
@@ -531,7 +531,7 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>700</v>
@@ -557,7 +557,7 @@
         <v>0.7</v>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>700</v>
@@ -583,7 +583,7 @@
         <v>0.8</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>700</v>
@@ -609,7 +609,7 @@
         <v>0.9</v>
       </c>
       <c r="C5">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>700</v>
@@ -635,7 +635,7 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>600</v>
@@ -661,7 +661,7 @@
         <v>0.7</v>
       </c>
       <c r="C7">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>600</v>
@@ -687,7 +687,7 @@
         <v>0.8</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>600</v>
@@ -713,7 +713,7 @@
         <v>0.9</v>
       </c>
       <c r="C9">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>600</v>
@@ -739,7 +739,7 @@
         <v>0.5</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>900</v>
@@ -765,7 +765,7 @@
         <v>0.7</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>900</v>
@@ -791,7 +791,7 @@
         <v>0.8</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>900</v>
@@ -817,7 +817,7 @@
         <v>0.9</v>
       </c>
       <c r="C13">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="D13">
         <v>900</v>
@@ -843,7 +843,7 @@
         <v>0.5</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>800</v>
@@ -869,7 +869,7 @@
         <v>0.7</v>
       </c>
       <c r="C15">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>800</v>
@@ -895,7 +895,7 @@
         <v>0.8</v>
       </c>
       <c r="C16">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>800</v>
@@ -921,7 +921,7 @@
         <v>0.9</v>
       </c>
       <c r="C17">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D17">
         <v>800</v>
@@ -947,7 +947,7 @@
         <v>0.5</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>800</v>
@@ -973,7 +973,7 @@
         <v>0.7</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>800</v>
@@ -999,7 +999,7 @@
         <v>0.8</v>
       </c>
       <c r="C20">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>800</v>
@@ -1025,7 +1025,7 @@
         <v>0.9</v>
       </c>
       <c r="C21">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>800</v>
@@ -1077,7 +1077,7 @@
         <v>0.7</v>
       </c>
       <c r="C23">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>900</v>
@@ -1103,7 +1103,7 @@
         <v>0.8</v>
       </c>
       <c r="C24">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D24">
         <v>900</v>
@@ -1129,7 +1129,7 @@
         <v>0.9</v>
       </c>
       <c r="C25">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D25">
         <v>900</v>
@@ -1155,7 +1155,7 @@
         <v>0.5</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>700</v>
@@ -1181,7 +1181,7 @@
         <v>0.7</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>700</v>
@@ -1207,7 +1207,7 @@
         <v>0.8</v>
       </c>
       <c r="C28">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>700</v>
@@ -1233,7 +1233,7 @@
         <v>0.9</v>
       </c>
       <c r="C29">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>700</v>
@@ -1259,7 +1259,7 @@
         <v>0.5</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>600</v>
@@ -1285,7 +1285,7 @@
         <v>0.7</v>
       </c>
       <c r="C31">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D31">
         <v>600</v>
@@ -1311,7 +1311,7 @@
         <v>0.8</v>
       </c>
       <c r="C32">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>600</v>
@@ -1337,7 +1337,7 @@
         <v>0.9</v>
       </c>
       <c r="C33">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>600</v>
@@ -1363,7 +1363,7 @@
         <v>0.5</v>
       </c>
       <c r="C34">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>800</v>
@@ -1389,7 +1389,7 @@
         <v>0.7</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D35">
         <v>800</v>
@@ -1415,7 +1415,7 @@
         <v>0.8</v>
       </c>
       <c r="C36">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>800</v>
@@ -1441,7 +1441,7 @@
         <v>0.9</v>
       </c>
       <c r="C37">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D37">
         <v>800</v>
@@ -1467,7 +1467,7 @@
         <v>0.5</v>
       </c>
       <c r="C38">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <v>900</v>
@@ -1493,7 +1493,7 @@
         <v>0.7</v>
       </c>
       <c r="C39">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D39">
         <v>900</v>
@@ -1519,7 +1519,7 @@
         <v>0.8</v>
       </c>
       <c r="C40">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D40">
         <v>900</v>
@@ -1545,7 +1545,7 @@
         <v>0.9</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="D41">
         <v>900</v>
@@ -1571,7 +1571,7 @@
         <v>0.5</v>
       </c>
       <c r="C42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D42">
         <v>700</v>
@@ -1597,7 +1597,7 @@
         <v>0.7</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D43">
         <v>700</v>
@@ -1623,7 +1623,7 @@
         <v>0.8</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D44">
         <v>700</v>
@@ -1649,7 +1649,7 @@
         <v>0.9</v>
       </c>
       <c r="C45">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D45">
         <v>700</v>
@@ -1675,7 +1675,7 @@
         <v>0.5</v>
       </c>
       <c r="C46">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46">
         <v>600</v>
@@ -1701,7 +1701,7 @@
         <v>0.7</v>
       </c>
       <c r="C47">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D47">
         <v>600</v>
@@ -1727,7 +1727,7 @@
         <v>0.8</v>
       </c>
       <c r="C48">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D48">
         <v>600</v>
@@ -1753,7 +1753,7 @@
         <v>0.9</v>
       </c>
       <c r="C49">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D49">
         <v>600</v>
@@ -1779,7 +1779,7 @@
         <v>0.5</v>
       </c>
       <c r="C50">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <v>700</v>
@@ -1805,7 +1805,7 @@
         <v>0.7</v>
       </c>
       <c r="C51">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D51">
         <v>700</v>
@@ -1831,7 +1831,7 @@
         <v>0.8</v>
       </c>
       <c r="C52">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D52">
         <v>700</v>
@@ -1857,7 +1857,7 @@
         <v>0.9</v>
       </c>
       <c r="C53">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D53">
         <v>700</v>
@@ -1883,7 +1883,7 @@
         <v>0.5</v>
       </c>
       <c r="C54">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D54">
         <v>800</v>
@@ -1909,7 +1909,7 @@
         <v>0.7</v>
       </c>
       <c r="C55">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D55">
         <v>800</v>
@@ -1935,7 +1935,7 @@
         <v>0.8</v>
       </c>
       <c r="C56">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D56">
         <v>800</v>
@@ -1961,7 +1961,7 @@
         <v>0.9</v>
       </c>
       <c r="C57">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="D57">
         <v>800</v>
@@ -1987,7 +1987,7 @@
         <v>0.5</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D58">
         <v>900</v>
@@ -2013,7 +2013,7 @@
         <v>0.7</v>
       </c>
       <c r="C59">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D59">
         <v>900</v>
@@ -2039,7 +2039,7 @@
         <v>0.8</v>
       </c>
       <c r="C60">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D60">
         <v>900</v>
@@ -2065,7 +2065,7 @@
         <v>0.9</v>
       </c>
       <c r="C61">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D61">
         <v>900</v>
@@ -2091,7 +2091,7 @@
         <v>0.5</v>
       </c>
       <c r="C62">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D62">
         <v>600</v>
@@ -2117,7 +2117,7 @@
         <v>0.7</v>
       </c>
       <c r="C63">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>600</v>
@@ -2143,7 +2143,7 @@
         <v>0.8</v>
       </c>
       <c r="C64">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D64">
         <v>600</v>
@@ -2169,7 +2169,7 @@
         <v>0.9</v>
       </c>
       <c r="C65">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D65">
         <v>600</v>
@@ -2195,7 +2195,7 @@
         <v>0.5</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D66">
         <v>900</v>
@@ -2221,7 +2221,7 @@
         <v>0.7</v>
       </c>
       <c r="C67">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="D67">
         <v>900</v>
@@ -2247,7 +2247,7 @@
         <v>0.8</v>
       </c>
       <c r="C68">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="D68">
         <v>900</v>
@@ -2273,7 +2273,7 @@
         <v>0.9</v>
       </c>
       <c r="C69">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="D69">
         <v>900</v>
@@ -2299,7 +2299,7 @@
         <v>0.5</v>
       </c>
       <c r="C70">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D70">
         <v>600</v>
@@ -2325,7 +2325,7 @@
         <v>0.7</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D71">
         <v>600</v>
@@ -2351,7 +2351,7 @@
         <v>0.8</v>
       </c>
       <c r="C72">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D72">
         <v>600</v>
@@ -2377,7 +2377,7 @@
         <v>0.9</v>
       </c>
       <c r="C73">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D73">
         <v>600</v>
@@ -2403,7 +2403,7 @@
         <v>0.5</v>
       </c>
       <c r="C74">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D74">
         <v>600</v>
@@ -2429,7 +2429,7 @@
         <v>0.7</v>
       </c>
       <c r="C75">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D75">
         <v>600</v>
@@ -2455,7 +2455,7 @@
         <v>0.8</v>
       </c>
       <c r="C76">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D76">
         <v>600</v>
@@ -2481,7 +2481,7 @@
         <v>0.9</v>
       </c>
       <c r="C77">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D77">
         <v>600</v>
@@ -2507,7 +2507,7 @@
         <v>0.5</v>
       </c>
       <c r="C78">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D78">
         <v>900</v>
@@ -2533,7 +2533,7 @@
         <v>0.7</v>
       </c>
       <c r="C79">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D79">
         <v>900</v>
@@ -2559,7 +2559,7 @@
         <v>0.8</v>
       </c>
       <c r="C80">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D80">
         <v>900</v>
@@ -2585,7 +2585,7 @@
         <v>0.9</v>
       </c>
       <c r="C81">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D81">
         <v>900</v>
@@ -2611,7 +2611,7 @@
         <v>0.5</v>
       </c>
       <c r="C82">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D82">
         <v>700</v>
@@ -2637,7 +2637,7 @@
         <v>0.7</v>
       </c>
       <c r="C83">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D83">
         <v>700</v>
@@ -2663,7 +2663,7 @@
         <v>0.8</v>
       </c>
       <c r="C84">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D84">
         <v>700</v>
@@ -2689,7 +2689,7 @@
         <v>0.9</v>
       </c>
       <c r="C85">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D85">
         <v>700</v>
@@ -2715,7 +2715,7 @@
         <v>0.5</v>
       </c>
       <c r="C86">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D86">
         <v>800</v>
@@ -2741,7 +2741,7 @@
         <v>0.7</v>
       </c>
       <c r="C87">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D87">
         <v>800</v>
@@ -2767,7 +2767,7 @@
         <v>0.8</v>
       </c>
       <c r="C88">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D88">
         <v>800</v>
@@ -2793,7 +2793,7 @@
         <v>0.9</v>
       </c>
       <c r="C89">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D89">
         <v>800</v>
@@ -2819,7 +2819,7 @@
         <v>0.5</v>
       </c>
       <c r="C90">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D90">
         <v>800</v>
@@ -2845,7 +2845,7 @@
         <v>0.7</v>
       </c>
       <c r="C91">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D91">
         <v>800</v>
@@ -2871,7 +2871,7 @@
         <v>0.8</v>
       </c>
       <c r="C92">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D92">
         <v>800</v>
@@ -2897,7 +2897,7 @@
         <v>0.9</v>
       </c>
       <c r="C93">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D93">
         <v>800</v>
@@ -2923,7 +2923,7 @@
         <v>0.5</v>
       </c>
       <c r="C94">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D94">
         <v>700</v>
@@ -2949,7 +2949,7 @@
         <v>0.7</v>
       </c>
       <c r="C95">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D95">
         <v>700</v>
@@ -2975,7 +2975,7 @@
         <v>0.8</v>
       </c>
       <c r="C96">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D96">
         <v>700</v>
@@ -3001,7 +3001,7 @@
         <v>0.9</v>
       </c>
       <c r="C97">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D97">
         <v>700</v>

</xml_diff>